<commit_message>
Created UI for View Data window; added functionality.
</commit_message>
<xml_diff>
--- a/Documentation.xlsx
+++ b/Documentation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projects\Repos\Process Times\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{199E63F8-3A42-4A30-AFB6-A61E47874834}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8897A5F6-B324-46E1-B557-8B749CCC4801}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D19486C0-902C-4885-ACEC-411A9C143975}"/>
   </bookViews>
@@ -132,9 +132,6 @@
     <t>3. Submit (button)</t>
   </si>
   <si>
-    <t>PROGRAM STRUCTURE</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">1. Summary (grid, </t>
     </r>
@@ -156,6 +153,9 @@
       </rPr>
       <t>)</t>
     </r>
+  </si>
+  <si>
+    <t>APPLICATION STRUCTURE</t>
   </si>
 </sst>
 </file>
@@ -1041,7 +1041,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{499C60A3-4568-4305-A203-E605168CB7E6}">
   <dimension ref="B1:M24"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1054,7 +1056,7 @@
   <sheetData>
     <row r="1" spans="2:13" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="13" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -1296,7 +1298,7 @@
       </c>
       <c r="E14" s="11"/>
       <c r="F14" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G14" s="11"/>
       <c r="H14" s="4" t="s">

</xml_diff>